<commit_message>
feat: add UI desktop
</commit_message>
<xml_diff>
--- a/src/main/resources/sample/Grade10_802910/B1_U1-8_SP/VWA_LevE_U1_SP.xlsx
+++ b/src/main/resources/sample/Grade10_802910/B1_U1-8_SP/VWA_LevE_U1_SP.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\.Data\G10\802910_IP_lvE_u1-8\802910_IP_lvE_u1-8\assets\resources\VWSA25_InsAndPrac_g10E\B1_U1-8_SP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaToolContentInput\ContentInput\src\main\resources\sample\Grade10_802910\B1_U1-8_SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="wordList" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="331">
   <si>
     <t>WordID</t>
   </si>
@@ -487,15 +487,6 @@
     <t>Step</t>
   </si>
   <si>
-    <t xml:space="preserve">Item Type </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Word</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inflected Forms Direction Line </t>
-  </si>
-  <si>
     <t>Inflected Forms</t>
   </si>
   <si>
@@ -530,9 +521,6 @@
   </si>
   <si>
     <t>Restate the definition(s) in your own words.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Draw or place a picture that is meaningful to you to help you quickly understand and remember the word. </t>
   </si>
   <si>
     <t>Adding an inflectional ending to a base word changes its number, degree, or tense.</t>
@@ -619,9 +607,6 @@
     <t>&lt;i&gt;artifices&lt;/i&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">a skillful or ingenious device; a clever trick or skill, trickery </t>
-  </si>
-  <si>
     <t>Even the most renowned art experts were completely taken in by the forger's [FIB: anno: artifice].</t>
   </si>
   <si>
@@ -685,36 +670,6 @@
   </si>
   <si>
     <t>to clarify, explain</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>The precise meaning of this passage in the novel</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>is sometimes hard to [FIB: anno: elucidate].</t>
-    </r>
   </si>
   <si>
     <t>elucidate</t>
@@ -1057,42 +1012,6 @@
     <t>9-10.L.4.c, 9-10.L.4.d</t>
   </si>
   <si>
-    <t>007724633</t>
-  </si>
-  <si>
-    <t>007724637</t>
-  </si>
-  <si>
-    <t>007724636</t>
-  </si>
-  <si>
-    <t>007724632</t>
-  </si>
-  <si>
-    <t>007724645</t>
-  </si>
-  <si>
-    <t>007724641</t>
-  </si>
-  <si>
-    <t>007724635</t>
-  </si>
-  <si>
-    <t>007724634</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I worked hard to [FIB: anno: redress] the harm I had caused. </t>
-  </si>
-  <si>
-    <t>007724642</t>
-  </si>
-  <si>
-    <t>007724646</t>
-  </si>
-  <si>
-    <t>007724639</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Remiss&lt;/b&gt; is an adjective that is used to describe someone who is "neglectful in performing a duty, careless."</t>
   </si>
   <si>
@@ -1121,6 +1040,24 @@
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>Item Type</t>
+  </si>
+  <si>
+    <t>Inflected Forms Direction Line</t>
+  </si>
+  <si>
+    <t>Draw or place a picture that is meaningful to you to help you quickly understand and remember the word.</t>
+  </si>
+  <si>
+    <t>a skillful or ingenious device; a clever trick or skill, trickery</t>
+  </si>
+  <si>
+    <t>I worked hard to [FIB: anno: redress] the harm I had caused.</t>
+  </si>
+  <si>
+    <t>The precise meaning of this passage in the novel is sometimes hard to [FIB: anno: elucidate].</t>
   </si>
 </sst>
 </file>
@@ -1584,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H13" sqref="A1:P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -1614,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -30334,24 +30271,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="17" customFormat="1">
       <c r="A1" s="17" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="90">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -30386,24 +30323,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="17" customFormat="1">
       <c r="A1" s="17" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="63">
       <c r="A2" s="14" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -30426,24 +30363,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="17" customFormat="1">
       <c r="A1" s="17" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="78.75">
       <c r="A2" s="14" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -30469,19 +30406,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="31" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="47.25">
       <c r="A2" s="33" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="35"/>
@@ -30496,9 +30433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" sqref="A1:R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -30521,13 +30458,13 @@
         <v>147</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>148</v>
+        <v>325</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>149</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -30536,16 +30473,16 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>150</v>
+        <v>326</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
@@ -30554,22 +30491,22 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -30582,10 +30519,10 @@
     </row>
     <row r="2" spans="1:26" ht="47.25">
       <c r="A2" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -30602,10 +30539,10 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>24</v>
@@ -30618,16 +30555,16 @@
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>321</v>
+        <v>159</v>
+      </c>
+      <c r="P2" s="19">
+        <v>7724633</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -30640,10 +30577,10 @@
     </row>
     <row r="3" spans="1:26" ht="94.5">
       <c r="A3" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>27</v>
@@ -30658,16 +30595,16 @@
         <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>31</v>
@@ -30680,16 +30617,16 @@
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>322</v>
+        <v>159</v>
+      </c>
+      <c r="P3" s="19">
+        <v>7724637</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
@@ -30702,10 +30639,10 @@
     </row>
     <row r="4" spans="1:26" ht="47.25">
       <c r="A4" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -30722,10 +30659,10 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>37</v>
@@ -30738,16 +30675,16 @@
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P4" s="19" t="s">
-        <v>321</v>
+        <v>159</v>
+      </c>
+      <c r="P4" s="19">
+        <v>7724633</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -30760,10 +30697,10 @@
     </row>
     <row r="5" spans="1:26" ht="63">
       <c r="A5" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>39</v>
@@ -30780,10 +30717,10 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>43</v>
@@ -30796,16 +30733,16 @@
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>322</v>
+        <v>159</v>
+      </c>
+      <c r="P5" s="19">
+        <v>7724637</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
@@ -30818,10 +30755,10 @@
     </row>
     <row r="6" spans="1:26" ht="47.25">
       <c r="A6" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>45</v>
@@ -30838,10 +30775,10 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>49</v>
@@ -30854,16 +30791,16 @@
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>323</v>
+        <v>159</v>
+      </c>
+      <c r="P6" s="19">
+        <v>7724636</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
@@ -30876,10 +30813,10 @@
     </row>
     <row r="7" spans="1:26" ht="47.25">
       <c r="A7" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>51</v>
@@ -30896,10 +30833,10 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>55</v>
@@ -30912,16 +30849,16 @@
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>324</v>
+        <v>159</v>
+      </c>
+      <c r="P7" s="19">
+        <v>7724632</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
@@ -30934,16 +30871,16 @@
     </row>
     <row r="8" spans="1:26" ht="94.5">
       <c r="A8" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>61</v>
@@ -30952,16 +30889,16 @@
         <v>62</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>64</v>
@@ -30970,20 +30907,20 @@
         <v>65</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P8" s="19" t="s">
-        <v>325</v>
+        <v>159</v>
+      </c>
+      <c r="P8" s="19">
+        <v>7724645</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
@@ -30996,16 +30933,16 @@
     </row>
     <row r="9" spans="1:26" ht="94.5">
       <c r="A9" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>68</v>
@@ -31014,16 +30951,16 @@
         <v>62</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>70</v>
@@ -31032,20 +30969,20 @@
         <v>71</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P9" s="19" t="s">
-        <v>326</v>
+        <v>159</v>
+      </c>
+      <c r="P9" s="19">
+        <v>7724641</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
@@ -31058,16 +30995,16 @@
     </row>
     <row r="10" spans="1:26" ht="94.5">
       <c r="A10" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>74</v>
@@ -31076,16 +31013,16 @@
         <v>75</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>77</v>
@@ -31094,20 +31031,20 @@
         <v>78</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P10" s="19" t="s">
-        <v>326</v>
+        <v>159</v>
+      </c>
+      <c r="P10" s="19">
+        <v>7724641</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
@@ -31120,16 +31057,16 @@
     </row>
     <row r="11" spans="1:26" ht="63">
       <c r="A11" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>81</v>
@@ -31140,10 +31077,10 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>83</v>
@@ -31152,20 +31089,20 @@
         <v>84</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P11" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="P11" s="19">
+        <v>7724635</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="Q11" s="7" t="s">
-        <v>163</v>
-      </c>
       <c r="R11" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
@@ -31178,10 +31115,10 @@
     </row>
     <row r="12" spans="1:26" ht="94.5">
       <c r="A12" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>85</v>
@@ -31196,16 +31133,16 @@
         <v>75</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>192</v>
+        <v>328</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>90</v>
@@ -31218,16 +31155,16 @@
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>328</v>
+        <v>159</v>
+      </c>
+      <c r="P12" s="19">
+        <v>7724634</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
@@ -31240,10 +31177,10 @@
     </row>
     <row r="13" spans="1:26" ht="63">
       <c r="A13" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>92</v>
@@ -31260,10 +31197,10 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>96</v>
@@ -31276,16 +31213,16 @@
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P13" s="19" t="s">
-        <v>323</v>
+        <v>159</v>
+      </c>
+      <c r="P13" s="19">
+        <v>7724636</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
@@ -31298,10 +31235,10 @@
     </row>
     <row r="14" spans="1:26" ht="47.25">
       <c r="A14" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>98</v>
@@ -31317,13 +31254,13 @@
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="J14" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>103</v>
@@ -31336,16 +31273,16 @@
       </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>325</v>
+        <v>159</v>
+      </c>
+      <c r="P14" s="19">
+        <v>7724645</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
@@ -31358,10 +31295,10 @@
     </row>
     <row r="15" spans="1:26" ht="47.25">
       <c r="A15" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>105</v>
@@ -31378,10 +31315,10 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>109</v>
@@ -31394,16 +31331,16 @@
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P15" s="19" t="s">
-        <v>328</v>
+        <v>159</v>
+      </c>
+      <c r="P15" s="19">
+        <v>7724634</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
@@ -31416,10 +31353,10 @@
     </row>
     <row r="16" spans="1:26" ht="94.5">
       <c r="A16" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>110</v>
@@ -31434,13 +31371,13 @@
         <v>62</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>329</v>
@@ -31456,16 +31393,16 @@
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P16" s="20" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
@@ -31478,10 +31415,10 @@
     </row>
     <row r="17" spans="1:26" ht="94.5">
       <c r="A17" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>116</v>
@@ -31496,16 +31433,16 @@
         <v>75</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>78</v>
@@ -31518,16 +31455,16 @@
       </c>
       <c r="N17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P17" s="20" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
@@ -31540,10 +31477,10 @@
     </row>
     <row r="18" spans="1:26" ht="94.5">
       <c r="A18" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>118</v>
@@ -31558,16 +31495,16 @@
         <v>75</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>122</v>
@@ -31580,16 +31517,16 @@
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>326</v>
+        <v>159</v>
+      </c>
+      <c r="P18" s="19">
+        <v>7724641</v>
       </c>
       <c r="Q18" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
@@ -31602,16 +31539,16 @@
     </row>
     <row r="19" spans="1:26" ht="47.25">
       <c r="A19" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>123</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>125</v>
@@ -31622,10 +31559,10 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="11" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>127</v>
@@ -31634,20 +31571,20 @@
         <v>128</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>330</v>
+        <v>159</v>
+      </c>
+      <c r="P19" s="19">
+        <v>7724642</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
@@ -31660,16 +31597,16 @@
     </row>
     <row r="20" spans="1:26" ht="94.5">
       <c r="A20" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>129</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>131</v>
@@ -31678,16 +31615,16 @@
         <v>62</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>214</v>
+        <v>330</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>133</v>
@@ -31696,20 +31633,20 @@
         <v>134</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>325</v>
+        <v>159</v>
+      </c>
+      <c r="P20" s="19">
+        <v>7724645</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
@@ -31722,16 +31659,16 @@
     </row>
     <row r="21" spans="1:26" ht="94.5">
       <c r="A21" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>135</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>137</v>
@@ -31740,16 +31677,16 @@
         <v>75</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>139</v>
@@ -31758,20 +31695,20 @@
         <v>140</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>331</v>
+        <v>159</v>
+      </c>
+      <c r="P21" s="19">
+        <v>7724646</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
@@ -31784,16 +31721,16 @@
     </row>
     <row r="22" spans="1:26" ht="47.25">
       <c r="A22" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>141</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>143</v>
@@ -31804,10 +31741,10 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>145</v>
@@ -31816,20 +31753,20 @@
         <v>146</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="P22" s="19" t="s">
-        <v>332</v>
+        <v>159</v>
+      </c>
+      <c r="P22" s="19">
+        <v>7724639</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
@@ -59263,13 +59200,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="72" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>5</v>
@@ -59281,46 +59218,46 @@
         <v>8</v>
       </c>
       <c r="G1" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="M1" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="N1" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="O1" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="P1" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="R1" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="S1" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>237</v>
-      </c>
       <c r="T1" s="22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="U1" s="22"/>
       <c r="V1" s="22"/>
@@ -59331,7 +59268,7 @@
     </row>
     <row r="2" spans="1:26" ht="99.75" customHeight="1">
       <c r="A2" s="20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -59350,33 +59287,33 @@
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="27" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
       <c r="S2" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
@@ -59403,7 +59340,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>8</v>
@@ -59412,27 +59349,27 @@
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="20" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="O3" s="20"/>
       <c r="P3" s="20" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="R3" s="20"/>
       <c r="S3" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
@@ -59460,37 +59397,37 @@
       </c>
       <c r="G4" s="26"/>
       <c r="H4" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
       <c r="L4" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="R4" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="M4" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>255</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>256</v>
-      </c>
       <c r="S4" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T4" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U4" s="23"/>
       <c r="V4" s="23"/>
@@ -59518,33 +59455,33 @@
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="27" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="20"/>
       <c r="S5" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T5" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U5" s="23"/>
       <c r="V5" s="23"/>
@@ -59578,27 +59515,27 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="O6" s="20"/>
       <c r="P6" s="20" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="R6" s="20"/>
       <c r="S6" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U6" s="23"/>
       <c r="V6" s="23"/>
@@ -59632,27 +59569,27 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="O7" s="20"/>
       <c r="P7" s="20" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="Q7" s="20" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="R7" s="20"/>
       <c r="S7" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T7" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U7" s="23"/>
       <c r="V7" s="23"/>
@@ -59679,40 +59616,40 @@
         <v>75</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="R8" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="M8" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="N8" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="O8" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="P8" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q8" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="R8" s="29" t="s">
-        <v>275</v>
-      </c>
       <c r="S8" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T8" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U8" s="23"/>
       <c r="V8" s="23"/>
@@ -59746,27 +59683,27 @@
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" s="28" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="M9" s="29" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="N9" s="29" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="O9" s="29"/>
       <c r="P9" s="20" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="Q9" s="29" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="R9" s="29"/>
       <c r="S9" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T9" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U9" s="23"/>
       <c r="V9" s="23"/>
@@ -59800,27 +59737,27 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="O10" s="20"/>
       <c r="P10" s="20" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="R10" s="20"/>
       <c r="S10" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T10" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U10" s="23"/>
       <c r="V10" s="23"/>
@@ -59848,33 +59785,33 @@
       </c>
       <c r="G11" s="26"/>
       <c r="H11" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="27" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="L11" s="28" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="O11" s="20"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
       <c r="R11" s="20"/>
       <c r="S11" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T11" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U11" s="23"/>
       <c r="V11" s="23"/>
@@ -59901,7 +59838,7 @@
         <v>62</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H12" s="20" t="s">
         <v>8</v>
@@ -59910,27 +59847,27 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
       <c r="L12" s="28" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="O12" s="20"/>
       <c r="P12" s="20" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="Q12" s="20" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="R12" s="20"/>
       <c r="S12" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T12" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U12" s="23"/>
       <c r="V12" s="23"/>
@@ -59957,7 +59894,7 @@
         <v>75</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H13" s="20" t="s">
         <v>8</v>
@@ -59966,27 +59903,27 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="O13" s="20"/>
       <c r="P13" s="20" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="R13" s="20"/>
       <c r="S13" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T13" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
@@ -60013,38 +59950,38 @@
         <v>75</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="O14" s="20"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
       <c r="S14" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="T14" s="20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="U14" s="23"/>
       <c r="V14" s="23"/>

</xml_diff>